<commit_message>
after all latest update
</commit_message>
<xml_diff>
--- a/src/test/resources/DieticianAPI.xlsx
+++ b/src/test/resources/DieticianAPI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meena\Eclipse-Dietician\APIDietician\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23E50F4-D8D8-4E95-98D9-78D33B754D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F32C52-33EF-467C-BD2C-1F3D73DD5BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="5" xr2:uid="{C4EDB30F-70E9-4635-AD8E-A92AAC9029B6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="6" xr2:uid="{C4EDB30F-70E9-4635-AD8E-A92AAC9029B6}"/>
   </bookViews>
   <sheets>
     <sheet name="GetAllmorbidity" sheetId="3" r:id="rId1"/>
@@ -923,12 +923,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11CB5494-7B58-4B34-A026-C532A127B7C6}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
@@ -1226,7 +1227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59E33E0A-BDCA-4B97-B43D-5CE62086FAB1}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>

</xml_diff>